<commit_message>
Tweaking to various modules in connection with subject-choice data. Also changed the base page for logged-in sessions (dispatch).
</commit_message>
<xml_diff>
--- a/TestData/Schuljahre/SCHULJAHR_2016/Schuldaten/Kurswahl/new/Kurswahl_13.xlsx
+++ b/TestData/Schuljahre/SCHULJAHR_2016/Schuldaten/Kurswahl/new/Kurswahl_13.xlsx
@@ -493,7 +493,7 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
       <selection activeCell="E1" activeCellId="0" pane="topRight" sqref="E1"/>
       <selection activeCell="A8" activeCellId="0" pane="bottomLeft" sqref="A8"/>
-      <selection activeCell="B8" activeCellId="0" pane="bottomRight" sqref="B8"/>
+      <selection activeCell="E8" activeCellId="0" pane="bottomRight" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8" outlineLevelRow="0" zeroHeight="0"/>
@@ -744,49 +744,29 @@
         </is>
       </c>
       <c r="D8" s="18" t="n"/>
-      <c r="E8" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="F8" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G8" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H8" s="22" t="inlineStr"/>
-      <c r="I8" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="J8" s="22" t="inlineStr"/>
-      <c r="K8" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="L8" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="M8" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="N8" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="O8" s="22" t="inlineStr"/>
+      <c r="E8" s="22" t="inlineStr"/>
+      <c r="F8" s="22" t="inlineStr"/>
+      <c r="G8" s="22" t="inlineStr"/>
+      <c r="H8" s="22" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="I8" s="22" t="inlineStr"/>
+      <c r="J8" s="22" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="K8" s="22" t="inlineStr"/>
+      <c r="L8" s="22" t="inlineStr"/>
+      <c r="M8" s="22" t="inlineStr"/>
+      <c r="N8" s="22" t="inlineStr"/>
+      <c r="O8" s="22" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="22.4" r="9" s="12">
       <c r="A9" s="17" t="inlineStr">
@@ -805,49 +785,29 @@
         </is>
       </c>
       <c r="D9" s="18" t="n"/>
-      <c r="E9" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="F9" s="22" t="inlineStr"/>
-      <c r="G9" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H9" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I9" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="J9" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="K9" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="L9" s="22" t="inlineStr"/>
-      <c r="M9" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="N9" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="O9" s="22" t="inlineStr"/>
+      <c r="E9" s="22" t="inlineStr"/>
+      <c r="F9" s="22" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="G9" s="22" t="inlineStr"/>
+      <c r="H9" s="22" t="inlineStr"/>
+      <c r="I9" s="22" t="inlineStr"/>
+      <c r="J9" s="22" t="inlineStr"/>
+      <c r="K9" s="22" t="inlineStr"/>
+      <c r="L9" s="22" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="M9" s="22" t="inlineStr"/>
+      <c r="N9" s="22" t="inlineStr"/>
+      <c r="O9" s="22" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="22.4" r="10" s="12">
       <c r="A10" s="17" t="inlineStr">
@@ -866,49 +826,29 @@
         </is>
       </c>
       <c r="D10" s="18" t="n"/>
-      <c r="E10" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="F10" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G10" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H10" s="22" t="inlineStr"/>
-      <c r="I10" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="J10" s="22" t="inlineStr"/>
-      <c r="K10" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="L10" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="M10" s="22" t="inlineStr"/>
-      <c r="N10" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="O10" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="E10" s="22" t="inlineStr"/>
+      <c r="F10" s="22" t="inlineStr"/>
+      <c r="G10" s="22" t="inlineStr"/>
+      <c r="H10" s="22" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="I10" s="22" t="inlineStr"/>
+      <c r="J10" s="22" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="K10" s="22" t="inlineStr"/>
+      <c r="L10" s="22" t="inlineStr"/>
+      <c r="M10" s="22" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N10" s="22" t="inlineStr"/>
+      <c r="O10" s="22" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="22.4" r="11" s="12">
       <c r="A11" s="17" t="inlineStr">
@@ -927,49 +867,29 @@
         </is>
       </c>
       <c r="D11" s="18" t="n"/>
-      <c r="E11" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="F11" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G11" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H11" s="22" t="inlineStr"/>
-      <c r="I11" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="J11" s="22" t="inlineStr"/>
-      <c r="K11" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="L11" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="M11" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="N11" s="22" t="inlineStr"/>
-      <c r="O11" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="E11" s="22" t="inlineStr"/>
+      <c r="F11" s="22" t="inlineStr"/>
+      <c r="G11" s="22" t="inlineStr"/>
+      <c r="H11" s="22" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="I11" s="22" t="inlineStr"/>
+      <c r="J11" s="22" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="K11" s="22" t="inlineStr"/>
+      <c r="L11" s="22" t="inlineStr"/>
+      <c r="M11" s="22" t="inlineStr"/>
+      <c r="N11" s="22" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="O11" s="22" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="22.4" r="12" s="12">
       <c r="A12" s="17" t="inlineStr">
@@ -988,49 +908,29 @@
         </is>
       </c>
       <c r="D12" s="18" t="n"/>
-      <c r="E12" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="F12" s="22" t="inlineStr"/>
-      <c r="G12" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H12" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I12" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="J12" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="K12" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="L12" s="22" t="inlineStr"/>
-      <c r="M12" s="22" t="inlineStr"/>
-      <c r="N12" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="O12" s="22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="E12" s="22" t="inlineStr"/>
+      <c r="F12" s="22" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="G12" s="22" t="inlineStr"/>
+      <c r="H12" s="22" t="inlineStr"/>
+      <c r="I12" s="22" t="inlineStr"/>
+      <c r="J12" s="22" t="inlineStr"/>
+      <c r="K12" s="22" t="inlineStr"/>
+      <c r="L12" s="22" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="M12" s="22" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N12" s="22" t="inlineStr"/>
+      <c r="O12" s="22" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="22.4" r="13" s="12"/>
     <row customHeight="1" ht="22.4" r="14" s="12"/>
@@ -1075,9 +975,9 @@
     <mergeCell ref="B1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="0" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1" sqref="E8:Z49" type="list">
-      <formula1>"X"</formula1>
-      <formula2>0</formula2>
+    <dataValidation allowBlank="0" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1" sqref="E8:Z49" type="textLength">
+      <formula1>0</formula1>
+      <formula2>5</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>

</xml_diff>